<commit_message>
Cleaned up and expanded logging test cases
</commit_message>
<xml_diff>
--- a/Payload Ops Tests/ExcelTests.xlsx
+++ b/Payload Ops Tests/ExcelTests.xlsx
@@ -73,6 +73,24 @@
   </x:si>
   <x:si>
     <x:t>1833</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1826</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5327</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8331</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4814</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2854</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8465</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -415,7 +433,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="K1" t="s">
-        <x:v>14</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -440,7 +458,7 @@
     </x:row>
     <x:row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <x:c r="A6" t="s">
-        <x:v>15</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="G6" t="s">
         <x:v>1</x:v>

</xml_diff>

<commit_message>
Updated spaceship and program to include logging
</commit_message>
<xml_diff>
--- a/Payload Ops Tests/ExcelTests.xlsx
+++ b/Payload Ops Tests/ExcelTests.xlsx
@@ -91,6 +91,18 @@
   </x:si>
   <x:si>
     <x:t>8465</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8838</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6514</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9552</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2824</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -433,7 +445,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="K1" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -458,7 +470,7 @@
     </x:row>
     <x:row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <x:c r="A6" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G6" t="s">
         <x:v>1</x:v>

</xml_diff>